<commit_message>
lendo colunas vazias no xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/files/excel.xlsx
+++ b/src/test/resources/files/excel.xlsx
@@ -15,16 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
-  <si>
-    <t>CNPJ</t>
-  </si>
-  <si>
-    <t>Razao_Social</t>
-  </si>
-  <si>
-    <t>Data_Emplacamento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>H1</t>
   </si>
@@ -33,15 +24,6 @@
   </si>
   <si>
     <t>H3</t>
-  </si>
-  <si>
-    <t>59104422002446</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN DO BRASIL LTDA</t>
-  </si>
-  <si>
-    <t>06/06/2013</t>
   </si>
   <si>
     <t>ABC</t>
@@ -53,25 +35,7 @@
     <t>GHI</t>
   </si>
   <si>
-    <t>03338422000160</t>
-  </si>
-  <si>
-    <t>AGULHAS NEGRAS DISTRIBUIDORA DE AUTOMOVEIS LTDA</t>
-  </si>
-  <si>
     <t>XXX</t>
-  </si>
-  <si>
-    <t>00208817000311</t>
-  </si>
-  <si>
-    <t>POWER IMPORTS VEICULOS LTDA</t>
-  </si>
-  <si>
-    <t>13280069000168</t>
-  </si>
-  <si>
-    <t>POWER MOTORS DISTRIB DE VEICULOS LTDA</t>
   </si>
 </sst>
 </file>
@@ -84,6 +48,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -145,12 +110,8 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -175,15 +136,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="P1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Q3" activeCellId="0" pane="topLeft" sqref="Q3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1048549" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -193,85 +157,25 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>